<commit_message>
++ update template + logic import invoice payment ở AR
</commit_message>
<xml_diff>
--- a/WebAPI/eFMS.API.SystemWeb/eFMS.API.Accounting/eFMS.API.Accounting/Resources/Files/InvoicePaymentImportTemplate.xlsx
+++ b/WebAPI/eFMS.API.SystemWeb/eFMS.API.Accounting/eFMS.API.Accounting/Resources/Files/InvoicePaymentImportTemplate.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Data\BA Project\Gitlab\eFMS\Tempate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kenny.thuong\Desktop\eFms\WebAPI\eFMS.API.SystemWeb\eFMS.API.Accounting\eFMS.API.Accounting\Resources\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t xml:space="preserve"> Partner Name</t>
   </si>
@@ -53,26 +53,35 @@
     <t>0000001</t>
   </si>
   <si>
-    <t>AE/20</t>
-  </si>
-  <si>
-    <t>UPS0999842</t>
-  </si>
-  <si>
-    <t>UPS VN</t>
-  </si>
-  <si>
     <t>Normal</t>
   </si>
   <si>
-    <t>Net Off</t>
+    <t>Currency*</t>
+  </si>
+  <si>
+    <t>Exchange Rate</t>
+  </si>
+  <si>
+    <t>Payment Method*</t>
+  </si>
+  <si>
+    <t>Cash</t>
+  </si>
+  <si>
+    <t>0100100181</t>
+  </si>
+  <si>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>VND</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -88,16 +97,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF212529"/>
+      <name val="Roboto"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF7F8FA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -120,16 +140,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -410,25 +442,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.7265625" customWidth="1"/>
-    <col min="2" max="2" width="11.453125" customWidth="1"/>
-    <col min="3" max="3" width="14.26953125" customWidth="1"/>
-    <col min="4" max="4" width="16.36328125" customWidth="1"/>
-    <col min="5" max="5" width="19.453125" customWidth="1"/>
-    <col min="6" max="6" width="13.7265625" customWidth="1"/>
-    <col min="7" max="7" width="14.6328125" customWidth="1"/>
-    <col min="8" max="8" width="14.1796875" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" customWidth="1"/>
+    <col min="8" max="8" width="21.28515625" customWidth="1"/>
+    <col min="9" max="9" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="15.75" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -445,66 +478,60 @@
         <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="B2" s="5">
+        <v>32332</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="3"/>
       <c r="E2" s="3">
         <v>2500000</v>
       </c>
-      <c r="F2" s="4">
-        <v>43999</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="3"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="F2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="3">
+        <v>1</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="4">
+        <v>44051</v>
+      </c>
+      <c r="J2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="3">
-        <v>2500000</v>
-      </c>
-      <c r="F3" s="4">
-        <v>43999</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="3"/>
+      <c r="K2" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2">
       <formula1>"Normal, Net Off"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>